<commit_message>
Fine draft of report done
</commit_message>
<xml_diff>
--- a/results/master_results.xlsx
+++ b/results/master_results.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B37CFED7-2A5E-4C02-AF20-9854FBBFF009}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C497DAA7-AC5F-4CCC-852E-D009B5836EA1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="7" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CHOI MRP" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="898" uniqueCount="215">
   <si>
     <t>injury and poisoning</t>
   </si>
@@ -522,94 +522,16 @@
     <t>Examples</t>
   </si>
   <si>
-    <t>Relative vs Mean</t>
-  </si>
-  <si>
-    <t>\blu{-0.043}</t>
-  </si>
-  <si>
-    <t>\blu{-0.301}</t>
-  </si>
-  <si>
-    <t>\blu{-0.459}</t>
-  </si>
-  <si>
-    <t>\ora{0.046}</t>
-  </si>
-  <si>
-    <t>\ora{0.007}</t>
-  </si>
-  <si>
-    <t>\blu{-0.274}</t>
-  </si>
-  <si>
-    <t>\blu{-0.016}</t>
-  </si>
-  <si>
-    <t>\blu{-0.154}</t>
-  </si>
-  <si>
-    <t>\blu{-0.368}</t>
-  </si>
-  <si>
-    <t>\ora{0.019}</t>
-  </si>
-  <si>
-    <t>\blu{-0.227}</t>
-  </si>
-  <si>
-    <t>\blu{-0.668}</t>
-  </si>
-  <si>
     <t>All Relevent Embeddings</t>
   </si>
   <si>
     <t>Overlapping Embeddings</t>
   </si>
   <si>
-    <t>\blu{-0.202}</t>
-  </si>
-  <si>
-    <t>\blu{-0.29}</t>
-  </si>
-  <si>
-    <t>\blu{-0.17}</t>
-  </si>
-  <si>
-    <t>\blu{-0.175}</t>
-  </si>
-  <si>
-    <t>\ora{0.027}</t>
-  </si>
-  <si>
-    <t>\blu{-0.559}</t>
-  </si>
-  <si>
-    <t>\blu{-0.283}</t>
-  </si>
-  <si>
-    <t>\blu{-0.064}</t>
-  </si>
-  <si>
-    <t>\blu{-0.098}</t>
-  </si>
-  <si>
-    <t>\blu{-0.555}</t>
-  </si>
-  <si>
-    <t>\blu{-0.498}</t>
-  </si>
-  <si>
-    <t>\blu{-0.569}</t>
-  </si>
-  <si>
     <t>T-test between overlapping and all</t>
   </si>
   <si>
     <t>Sig different?</t>
-  </si>
-  <si>
-    <t>Significant Difference?</t>
   </si>
   <si>
     <t>Yes</t>
@@ -622,6 +544,141 @@
   </si>
   <si>
     <t>Spearman:</t>
+  </si>
+  <si>
+    <t>\ora{22}</t>
+  </si>
+  <si>
+    <t>\blu{-20}</t>
+  </si>
+  <si>
+    <t>\blu{-29}</t>
+  </si>
+  <si>
+    <t>\blu{-34}</t>
+  </si>
+  <si>
+    <t>\ora{37}</t>
+  </si>
+  <si>
+    <t>\ora{30}</t>
+  </si>
+  <si>
+    <t>\ora{38}</t>
+  </si>
+  <si>
+    <t>\blu{-17}</t>
+  </si>
+  <si>
+    <t>\blu{-18}</t>
+  </si>
+  <si>
+    <t>\blu{-56}</t>
+  </si>
+  <si>
+    <t>\blu{-28}</t>
+  </si>
+  <si>
+    <t>\blu{-55}</t>
+  </si>
+  <si>
+    <t>\blu{-50}</t>
+  </si>
+  <si>
+    <t>\blu{-57}</t>
+  </si>
+  <si>
+    <t>Difference (\%)</t>
+  </si>
+  <si>
+    <t>Different?</t>
+  </si>
+  <si>
+    <t>\blu{-4}</t>
+  </si>
+  <si>
+    <t>\ora{12}</t>
+  </si>
+  <si>
+    <t>\blu{-30}</t>
+  </si>
+  <si>
+    <t>\blu{-46}</t>
+  </si>
+  <si>
+    <t>\ora{16}</t>
+  </si>
+  <si>
+    <t>\ora{5}</t>
+  </si>
+  <si>
+    <t>\blu{-27}</t>
+  </si>
+  <si>
+    <t>\blu{-15}</t>
+  </si>
+  <si>
+    <t>\ora{27}</t>
+  </si>
+  <si>
+    <t>\blu{-37}</t>
+  </si>
+  <si>
+    <t>\blu{-23}</t>
+  </si>
+  <si>
+    <t>\blu{-67}</t>
+  </si>
+  <si>
+    <t>\ora{13}</t>
+  </si>
+  <si>
+    <t>Cancers</t>
+  </si>
+  <si>
+    <t>Endocrine</t>
+  </si>
+  <si>
+    <t>Blood Diseases</t>
+  </si>
+  <si>
+    <t>Mental Disorders</t>
+  </si>
+  <si>
+    <t>Cardiovascular</t>
+  </si>
+  <si>
+    <t>Respiratory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genitourinary </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digestive </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nervous </t>
+  </si>
+  <si>
+    <t>Pregnancy</t>
+  </si>
+  <si>
+    <t>Skin</t>
+  </si>
+  <si>
+    <t>Muscoskeletal</t>
+  </si>
+  <si>
+    <t>Congenital Anomolies</t>
+  </si>
+  <si>
+    <t>Perinatal</t>
+  </si>
+  <si>
+    <t>Ill-defined</t>
+  </si>
+  <si>
+    <t>Injury and Poisoning</t>
   </si>
 </sst>
 </file>
@@ -1511,27 +1568,28 @@
   <dimension ref="A1:V1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.140625" customWidth="1"/>
+    <col min="1" max="1" width="30" customWidth="1"/>
     <col min="2" max="3" width="20.85546875" customWidth="1"/>
     <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="E1" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
         <v>160</v>
@@ -1540,7 +1598,7 @@
         <v>161</v>
       </c>
       <c r="D2" t="s">
-        <v>162</v>
+        <v>184</v>
       </c>
       <c r="E2" t="s">
         <v>102</v>
@@ -1549,36 +1607,38 @@
         <v>161</v>
       </c>
       <c r="G2" t="s">
-        <v>162</v>
+        <v>184</v>
       </c>
       <c r="H2" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B3" s="6">
-        <v>7.7222</v>
+        <v>8.0663797683636833</v>
       </c>
       <c r="C3">
-        <v>2261</v>
-      </c>
-      <c r="D3" t="s">
-        <v>163</v>
+        <f>SUM(C4:C20)</f>
+        <v>16351</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
       </c>
       <c r="E3" s="6">
-        <v>6.8430250362219347</v>
+        <v>5.5972693640028011</v>
       </c>
       <c r="F3">
-        <v>334</v>
+        <f>SUM(F4:F20)</f>
+        <v>2884</v>
       </c>
       <c r="G3">
-        <v>0.223</v>
+        <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>192</v>
+        <v>166</v>
       </c>
       <c r="N3" s="6">
         <v>7.7222</v>
@@ -1587,7 +1647,7 @@
         <v>6.8430250362219347</v>
       </c>
       <c r="P3" s="8">
-        <f>_xlfn.RANK.AVG(N3,$N$3:$N$19,0)</f>
+        <f t="shared" ref="P3:P19" si="0">_xlfn.RANK.AVG(N3,$N$3:$N$19,0)</f>
         <v>10</v>
       </c>
       <c r="Q3" s="8">
@@ -1604,28 +1664,28 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>106</v>
       </c>
       <c r="B4" s="6">
-        <v>9.0022000000000002</v>
+        <v>7.7221963698412797</v>
       </c>
       <c r="C4">
-        <v>1194</v>
-      </c>
-      <c r="D4">
-        <v>0.11600000000000001</v>
+        <v>2261</v>
+      </c>
+      <c r="D4" t="s">
+        <v>186</v>
       </c>
       <c r="E4" s="6">
-        <v>4.4677419593915282</v>
+        <v>6.8430250362219347</v>
       </c>
       <c r="F4">
-        <v>116</v>
+        <v>334</v>
       </c>
       <c r="G4" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="H4" t="s">
-        <v>192</v>
+        <v>166</v>
       </c>
       <c r="N4" s="6">
         <v>9.0022000000000002</v>
@@ -1634,11 +1694,11 @@
         <v>4.4677419593915282</v>
       </c>
       <c r="P4" s="8">
-        <f>_xlfn.RANK.AVG(N4,$N$3:$N$19,0)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="Q4" s="8">
-        <f t="shared" ref="Q4:Q19" si="0">_xlfn.RANK.AVG(O4,$O$3:$O$19,0)</f>
+        <f t="shared" ref="Q4:Q19" si="1">_xlfn.RANK.AVG(O4,$O$3:$O$19,0)</f>
         <v>10</v>
       </c>
       <c r="T4" s="3" t="s">
@@ -1651,28 +1711,28 @@
     </row>
     <row r="5" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>199</v>
       </c>
       <c r="B5" s="6">
-        <v>5.6385199999999998</v>
+        <v>9.0021952139878465</v>
       </c>
       <c r="C5">
-        <v>545</v>
+        <v>1194</v>
       </c>
       <c r="D5" t="s">
-        <v>164</v>
+        <v>187</v>
       </c>
       <c r="E5" s="6">
-        <v>3.9758853697661558</v>
+        <v>4.4677419593915282</v>
       </c>
       <c r="F5">
-        <v>193</v>
+        <v>116</v>
       </c>
       <c r="G5" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="H5" t="s">
-        <v>192</v>
+        <v>166</v>
       </c>
       <c r="N5" s="6">
         <v>5.6385199999999998</v>
@@ -1681,11 +1741,11 @@
         <v>3.9758853697661558</v>
       </c>
       <c r="P5" s="8">
-        <f>_xlfn.RANK.AVG(N5,$N$3:$N$19,0)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="Q5" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="T5" s="4" t="s">
@@ -1700,28 +1760,28 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>200</v>
       </c>
       <c r="B6" s="6">
-        <v>4.3599500000000004</v>
+        <v>5.6385226166830336</v>
       </c>
       <c r="C6">
-        <v>199</v>
+        <v>545</v>
       </c>
       <c r="D6" t="s">
-        <v>165</v>
+        <v>188</v>
       </c>
       <c r="E6" s="6">
-        <v>3.6669327969756744</v>
+        <v>3.9758853697661558</v>
       </c>
       <c r="F6">
-        <v>81</v>
+        <v>193</v>
       </c>
       <c r="G6" t="s">
-        <v>153</v>
+        <v>172</v>
       </c>
       <c r="H6" t="s">
-        <v>192</v>
+        <v>166</v>
       </c>
       <c r="N6" s="6">
         <v>4.3599500000000004</v>
@@ -1730,38 +1790,38 @@
         <v>3.6669327969756744</v>
       </c>
       <c r="P6" s="8">
-        <f>_xlfn.RANK.AVG(N6,$N$3:$N$19,0)</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="Q6" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>201</v>
       </c>
       <c r="B7" s="6">
-        <v>9.3376900000000003</v>
+        <v>4.3599470781903236</v>
       </c>
       <c r="C7">
-        <v>662</v>
-      </c>
-      <c r="D7">
-        <v>0.158</v>
+        <v>199</v>
+      </c>
+      <c r="D7" t="s">
+        <v>189</v>
       </c>
       <c r="E7" s="6">
-        <v>7.6720359017048683</v>
+        <v>3.6669327969756744</v>
       </c>
       <c r="F7">
-        <v>165</v>
-      </c>
-      <c r="G7">
-        <v>0.371</v>
+        <v>81</v>
+      </c>
+      <c r="G7" t="s">
+        <v>173</v>
       </c>
       <c r="H7" t="s">
-        <v>192</v>
+        <v>166</v>
       </c>
       <c r="N7" s="6">
         <v>9.3376900000000003</v>
@@ -1770,38 +1830,38 @@
         <v>7.6720359017048683</v>
       </c>
       <c r="P7" s="8">
-        <f>_xlfn.RANK.AVG(N7,$N$3:$N$19,0)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="Q7" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>202</v>
       </c>
       <c r="B8" s="6">
-        <v>8.4372799999999994</v>
+        <v>9.3376911803444536</v>
       </c>
       <c r="C8">
-        <v>1787</v>
+        <v>662</v>
       </c>
       <c r="D8" t="s">
+        <v>190</v>
+      </c>
+      <c r="E8" s="6">
+        <v>7.6720359017048683</v>
+      </c>
+      <c r="F8">
+        <v>165</v>
+      </c>
+      <c r="G8" t="s">
+        <v>174</v>
+      </c>
+      <c r="H8" t="s">
         <v>166</v>
-      </c>
-      <c r="E8" s="6">
-        <v>7.266461055114263</v>
-      </c>
-      <c r="F8">
-        <v>434</v>
-      </c>
-      <c r="G8">
-        <v>0.29799999999999999</v>
-      </c>
-      <c r="H8" t="s">
-        <v>192</v>
       </c>
       <c r="N8" s="6">
         <v>8.4372799999999994</v>
@@ -1810,38 +1870,38 @@
         <v>7.266461055114263</v>
       </c>
       <c r="P8" s="8">
-        <f>_xlfn.RANK.AVG(N8,$N$3:$N$19,0)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="Q8" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>207</v>
       </c>
       <c r="B9" s="6">
-        <v>8.1222700000000003</v>
+        <v>8.4372800574368174</v>
       </c>
       <c r="C9">
-        <v>869</v>
+        <v>1787</v>
       </c>
       <c r="D9" t="s">
-        <v>167</v>
+        <v>191</v>
       </c>
       <c r="E9" s="6">
-        <v>7.7403307054998551</v>
+        <v>7.266461055114263</v>
       </c>
       <c r="F9">
-        <v>307</v>
-      </c>
-      <c r="G9">
-        <v>0.38300000000000001</v>
+        <v>434</v>
+      </c>
+      <c r="G9" t="s">
+        <v>175</v>
       </c>
       <c r="H9" t="s">
-        <v>193</v>
+        <v>166</v>
       </c>
       <c r="N9" s="6">
         <v>8.1222700000000003</v>
@@ -1850,11 +1910,11 @@
         <v>7.7403307054998551</v>
       </c>
       <c r="P9" s="8">
-        <f>_xlfn.RANK.AVG(N9,$N$3:$N$19,0)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="Q9" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="T9" s="5"/>
@@ -1867,28 +1927,28 @@
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>203</v>
       </c>
       <c r="B10" s="6">
-        <v>5.85283</v>
+        <v>8.1222749690450549</v>
       </c>
       <c r="C10">
-        <v>405</v>
-      </c>
-      <c r="D10" t="s">
-        <v>168</v>
+        <v>869</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
       </c>
       <c r="E10" s="6">
-        <v>4.6443255395767364</v>
+        <v>7.7403307054998551</v>
       </c>
       <c r="F10">
-        <v>132</v>
+        <v>307</v>
       </c>
       <c r="G10" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H10" t="s">
-        <v>192</v>
+        <v>167</v>
       </c>
       <c r="N10" s="6">
         <v>5.85283</v>
@@ -1897,11 +1957,11 @@
         <v>4.6443255395767364</v>
       </c>
       <c r="P10" s="8">
-        <f>_xlfn.RANK.AVG(N10,$N$3:$N$19,0)</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="Q10" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="T10" s="3" t="s">
@@ -1915,28 +1975,28 @@
     </row>
     <row r="11" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>204</v>
       </c>
       <c r="B11" s="6">
-        <v>7.9349499999999997</v>
+        <v>5.852834801384919</v>
       </c>
       <c r="C11">
-        <v>852</v>
+        <v>405</v>
       </c>
       <c r="D11" t="s">
-        <v>169</v>
+        <v>192</v>
       </c>
       <c r="E11" s="6">
-        <v>4.6156940107140123</v>
+        <v>4.6443255395767364</v>
       </c>
       <c r="F11">
-        <v>210</v>
+        <v>132</v>
       </c>
       <c r="G11" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="H11" t="s">
-        <v>192</v>
+        <v>166</v>
       </c>
       <c r="N11" s="6">
         <v>7.9349499999999997</v>
@@ -1945,11 +2005,11 @@
         <v>4.6156940107140123</v>
       </c>
       <c r="P11" s="8">
-        <f>_xlfn.RANK.AVG(N11,$N$3:$N$19,0)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="Q11" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="T11" s="4" t="s">
@@ -1965,28 +2025,28 @@
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>206</v>
       </c>
       <c r="B12" s="6">
-        <v>6.8210899999999999</v>
+        <v>7.9349505481263813</v>
       </c>
       <c r="C12">
-        <v>606</v>
-      </c>
-      <c r="D12" t="s">
-        <v>170</v>
+        <v>852</v>
+      </c>
+      <c r="D12">
+        <v>-2</v>
       </c>
       <c r="E12" s="6">
-        <v>5.7470328225148117</v>
+        <v>4.6156940107140123</v>
       </c>
       <c r="F12">
         <v>210</v>
       </c>
       <c r="G12" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="H12" t="s">
-        <v>192</v>
+        <v>166</v>
       </c>
       <c r="N12" s="6">
         <v>6.8210899999999999</v>
@@ -1995,38 +2055,38 @@
         <v>5.7470328225148117</v>
       </c>
       <c r="P12" s="8">
-        <f>_xlfn.RANK.AVG(N12,$N$3:$N$19,0)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="Q12" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>205</v>
       </c>
       <c r="B13" s="6">
-        <v>10.26976</v>
+        <v>6.8210863324482149</v>
       </c>
       <c r="C13">
-        <v>1325</v>
-      </c>
-      <c r="D13">
-        <v>0.27300000000000002</v>
+        <v>606</v>
+      </c>
+      <c r="D13" t="s">
+        <v>193</v>
       </c>
       <c r="E13" s="6">
-        <v>2.4667761900182841</v>
+        <v>5.7470328225148117</v>
       </c>
       <c r="F13">
-        <v>10</v>
-      </c>
-      <c r="G13" t="s">
-        <v>182</v>
+        <v>210</v>
+      </c>
+      <c r="G13">
+        <v>3</v>
       </c>
       <c r="H13" t="s">
-        <v>192</v>
+        <v>166</v>
       </c>
       <c r="N13" s="6">
         <v>10.26976</v>
@@ -2035,38 +2095,38 @@
         <v>2.4667761900182841</v>
       </c>
       <c r="P13" s="8">
-        <f>_xlfn.RANK.AVG(N13,$N$3:$N$19,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="Q13" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>5</v>
+        <v>208</v>
       </c>
       <c r="B14" s="6">
-        <v>5.0997199999999996</v>
+        <v>10.269756919754551</v>
       </c>
       <c r="C14">
-        <v>305</v>
+        <v>1325</v>
       </c>
       <c r="D14" t="s">
-        <v>171</v>
+        <v>194</v>
       </c>
       <c r="E14" s="6">
-        <v>4.0136388428633794</v>
+        <v>2.4667761900182841</v>
       </c>
       <c r="F14">
-        <v>102</v>
+        <v>10</v>
       </c>
       <c r="G14" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="H14" t="s">
-        <v>192</v>
+        <v>166</v>
       </c>
       <c r="N14" s="6">
         <v>5.0997199999999996</v>
@@ -2075,15 +2135,15 @@
         <v>4.0136388428633794</v>
       </c>
       <c r="P14" s="8">
-        <f>_xlfn.RANK.AVG(N14,$N$3:$N$19,0)</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="Q14" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="S14" t="s">
-        <v>194</v>
+        <v>168</v>
       </c>
       <c r="T14">
         <f>PEARSON(N3:N19,O3:O19)</f>
@@ -2092,28 +2152,28 @@
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>4</v>
+        <v>209</v>
       </c>
       <c r="B15" s="6">
-        <v>8.2220200000000006</v>
+        <v>5.0997220123564384</v>
       </c>
       <c r="C15">
-        <v>1041</v>
+        <v>305</v>
       </c>
       <c r="D15" t="s">
-        <v>172</v>
+        <v>195</v>
       </c>
       <c r="E15" s="6">
-        <v>5.2414180480041113</v>
+        <v>4.0136388428633794</v>
       </c>
       <c r="F15">
-        <v>168</v>
+        <v>102</v>
       </c>
       <c r="G15" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="H15" t="s">
-        <v>192</v>
+        <v>166</v>
       </c>
       <c r="N15" s="6">
         <v>8.2220200000000006</v>
@@ -2122,15 +2182,15 @@
         <v>5.2414180480041113</v>
       </c>
       <c r="P15" s="8">
-        <f>_xlfn.RANK.AVG(N15,$N$3:$N$19,0)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="Q15" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="S15" t="s">
-        <v>195</v>
+        <v>169</v>
       </c>
       <c r="T15">
         <f>CORREL(P3:P19,Q3:Q19)</f>
@@ -2139,28 +2199,28 @@
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>3</v>
+        <v>210</v>
       </c>
       <c r="B16" s="6">
-        <v>6.2364300000000004</v>
+        <v>8.2220219138004023</v>
       </c>
       <c r="C16">
-        <v>457</v>
-      </c>
-      <c r="D16" t="s">
-        <v>173</v>
+        <v>1041</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
       </c>
       <c r="E16" s="6">
-        <v>5.0497655156784367</v>
+        <v>5.2414180480041113</v>
       </c>
       <c r="F16">
-        <v>101</v>
-      </c>
-      <c r="G16" t="s">
-        <v>185</v>
+        <v>168</v>
+      </c>
+      <c r="G16">
+        <v>-6</v>
       </c>
       <c r="H16" t="s">
-        <v>192</v>
+        <v>166</v>
       </c>
       <c r="N16" s="6">
         <v>6.2364300000000004</v>
@@ -2169,38 +2229,38 @@
         <v>5.0497655156784367</v>
       </c>
       <c r="P16" s="8">
-        <f>_xlfn.RANK.AVG(N16,$N$3:$N$19,0)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="Q16" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>2</v>
+        <v>211</v>
       </c>
       <c r="B17" s="6">
-        <v>9.8391300000000008</v>
+        <v>6.23642545462382</v>
       </c>
       <c r="C17">
-        <v>310</v>
-      </c>
-      <c r="D17">
-        <v>0.22</v>
+        <v>457</v>
+      </c>
+      <c r="D17" t="s">
+        <v>196</v>
       </c>
       <c r="E17" s="6">
-        <v>2.4931642859137186</v>
+        <v>5.0497655156784367</v>
       </c>
       <c r="F17">
-        <v>11</v>
-      </c>
-      <c r="G17" t="s">
-        <v>186</v>
+        <v>101</v>
+      </c>
+      <c r="G17">
+        <v>-10</v>
       </c>
       <c r="H17" t="s">
-        <v>192</v>
+        <v>166</v>
       </c>
       <c r="N17" s="6">
         <v>9.8391300000000008</v>
@@ -2209,38 +2269,38 @@
         <v>2.4931642859137186</v>
       </c>
       <c r="P17" s="8">
-        <f>_xlfn.RANK.AVG(N17,$N$3:$N$19,0)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="Q17" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>1</v>
+        <v>212</v>
       </c>
       <c r="B18" s="6">
-        <v>2.67645</v>
+        <v>9.8391250648607933</v>
       </c>
       <c r="C18">
-        <v>558</v>
+        <v>310</v>
       </c>
       <c r="D18" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E18" s="6">
-        <v>2.8103416848946741</v>
+        <v>2.4931642859137186</v>
       </c>
       <c r="F18">
-        <v>224</v>
+        <v>11</v>
       </c>
       <c r="G18" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="H18" t="s">
-        <v>193</v>
+        <v>166</v>
       </c>
       <c r="N18" s="6">
         <v>2.67645</v>
@@ -2249,38 +2309,38 @@
         <v>2.8103416848946741</v>
       </c>
       <c r="P18" s="8">
-        <f>_xlfn.RANK.AVG(N18,$N$3:$N$19,0)</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="Q18" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>0</v>
+        <v>213</v>
       </c>
       <c r="B19" s="6">
-        <v>9.0913799999999991</v>
+        <v>2.6764515603323926</v>
       </c>
       <c r="C19">
-        <v>2975</v>
-      </c>
-      <c r="D19">
-        <v>0.127</v>
+        <v>558</v>
+      </c>
+      <c r="D19" t="s">
+        <v>197</v>
       </c>
       <c r="E19" s="6">
-        <v>2.4152210628280666</v>
+        <v>2.8103416848946741</v>
       </c>
       <c r="F19">
-        <v>86</v>
+        <v>224</v>
       </c>
       <c r="G19" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="H19" t="s">
-        <v>192</v>
+        <v>167</v>
       </c>
       <c r="N19" s="6">
         <v>9.0913799999999991</v>
@@ -2289,12 +2349,38 @@
         <v>2.4152210628280666</v>
       </c>
       <c r="P19" s="8">
-        <f>_xlfn.RANK.AVG(N19,$N$3:$N$19,0)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="Q19" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>214</v>
+      </c>
+      <c r="B20" s="6">
+        <v>9.0913811262973745</v>
+      </c>
+      <c r="C20">
+        <v>2975</v>
+      </c>
+      <c r="D20" t="s">
+        <v>198</v>
+      </c>
+      <c r="E20" s="6">
+        <v>2.4152210628280666</v>
+      </c>
+      <c r="F20">
+        <v>86</v>
+      </c>
+      <c r="G20" t="s">
+        <v>183</v>
+      </c>
+      <c r="H20" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="1048576" spans="16:16" x14ac:dyDescent="0.25">
@@ -9503,7 +9589,7 @@
         <v>10.838392857142864</v>
       </c>
       <c r="AN6" t="b">
-        <f t="shared" ref="AN5:AN7" si="30">AL6&lt;0.05</f>
+        <f t="shared" ref="AN6:AN7" si="30">AL6&lt;0.05</f>
         <v>1</v>
       </c>
       <c r="AO6" s="6">
@@ -16783,8 +16869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF7A4162-D858-4318-9E51-5203B387E49B}">
   <dimension ref="A1:DJK40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R32" sqref="R32"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="M40" sqref="M23:M40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -65898,6 +65984,12 @@
         <f>AVERAGE(A1:DJK17)</f>
         <v>8.0663797683636833</v>
       </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="1:2975" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -65908,20 +66000,20 @@
         <v>7.7221963698412797</v>
       </c>
       <c r="J24">
-        <f>(I24-$I$23)/$I$23</f>
-        <v>-4.2668881010573027E-2</v>
+        <f>100*ROUND((I24-$I$23)/$I$23,2)</f>
+        <v>-4</v>
       </c>
       <c r="K24">
-        <f>_xlfn.T.TEST(1:1,$A$1:$DJK$17,2,3)</f>
+        <f t="shared" ref="K24:K40" si="0">_xlfn.T.TEST(1:1,$A$1:$DJK$17,2,3)</f>
         <v>3.2422405619458704E-6</v>
       </c>
       <c r="L24" t="b">
-        <f>J24&lt;0.05</f>
+        <f>K24&lt;0.05</f>
         <v>1</v>
       </c>
       <c r="M24" t="str">
-        <f>IF(AND(L24,J24&gt;0),"\ora{"&amp;ROUND(J24,3)&amp;"}",IF(AND(L24,J24&lt;0),"\blu{"&amp;ROUND(J24,3)&amp;"}",ROUND(J24,3)))</f>
-        <v>\blu{-0.043}</v>
+        <f>IF(AND(L24,J24&gt;0),"\ora{"&amp;J24&amp;"}",IF(AND(L24,J24&lt;0),"\blu{"&amp;J24&amp;"}",J24))</f>
+        <v>\blu{-4}</v>
       </c>
     </row>
     <row r="25" spans="1:2975" x14ac:dyDescent="0.25">
@@ -65929,24 +66021,24 @@
         <v>15</v>
       </c>
       <c r="I25">
-        <f t="shared" ref="I25:I40" si="0">AVERAGE(2:2)</f>
+        <f t="shared" ref="I25:I39" si="1">AVERAGE(2:2)</f>
         <v>9.0021952139878465</v>
       </c>
       <c r="J25">
-        <f t="shared" ref="J25:J40" si="1">(I25-$I$23)/$I$23</f>
-        <v>0.11601430536340832</v>
+        <f>100*ROUND((I25-$I$23)/$I$23,2)</f>
+        <v>12</v>
       </c>
       <c r="K25">
-        <f>_xlfn.T.TEST(2:2,$A$1:$DJK$17,2,3)</f>
+        <f t="shared" si="0"/>
         <v>2.6822004460146442E-26</v>
       </c>
       <c r="L25" t="b">
-        <f>J25&lt;0.05</f>
-        <v>0</v>
-      </c>
-      <c r="M25">
-        <f>IF(AND(L25,J25&gt;0),"\ora{"&amp;ROUND(J25,3)&amp;"}",IF(AND(L25,J25&lt;0),"\blu{"&amp;ROUND(J25,3)&amp;"}",ROUND(J25,3)))</f>
-        <v>0.11600000000000001</v>
+        <f t="shared" ref="L25:L40" si="2">K25&lt;0.05</f>
+        <v>1</v>
+      </c>
+      <c r="M25" t="str">
+        <f t="shared" ref="M25:M40" si="3">IF(AND(L25,J25&gt;0),"\ora{"&amp;J25&amp;"}",IF(AND(L25,J25&lt;0),"\blu{"&amp;J25&amp;"}",J25))</f>
+        <v>\ora{12}</v>
       </c>
     </row>
     <row r="26" spans="1:2975" x14ac:dyDescent="0.25">
@@ -65954,24 +66046,24 @@
         <v>14</v>
       </c>
       <c r="I26">
+        <f t="shared" si="1"/>
+        <v>5.6385226166830336</v>
+      </c>
+      <c r="J26">
+        <f>100*ROUND((I26-$I$23)/$I$23,2)</f>
+        <v>-30</v>
+      </c>
+      <c r="K26">
         <f t="shared" si="0"/>
-        <v>5.6385226166830336</v>
-      </c>
-      <c r="J26">
-        <f t="shared" si="1"/>
-        <v>-0.30098473186232788</v>
-      </c>
-      <c r="K26">
-        <f>_xlfn.T.TEST(3:3,$A$1:$DJK$17,2,3)</f>
         <v>4.4829982785094439E-60</v>
       </c>
       <c r="L26" t="b">
-        <f>J26&lt;0.05</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="M26" t="str">
-        <f>IF(AND(L26,J26&gt;0),"\ora{"&amp;ROUND(J26,3)&amp;"}",IF(AND(L26,J26&lt;0),"\blu{"&amp;ROUND(J26,3)&amp;"}",ROUND(J26,3)))</f>
-        <v>\blu{-0.301}</v>
+        <f t="shared" si="3"/>
+        <v>\blu{-30}</v>
       </c>
     </row>
     <row r="27" spans="1:2975" x14ac:dyDescent="0.25">
@@ -65979,24 +66071,24 @@
         <v>13</v>
       </c>
       <c r="I27">
+        <f t="shared" si="1"/>
+        <v>4.3599470781903236</v>
+      </c>
+      <c r="J27">
+        <f t="shared" ref="J27:J40" si="4">100*ROUND((I27-$I$23)/$I$23,2)</f>
+        <v>-46</v>
+      </c>
+      <c r="K27">
         <f t="shared" si="0"/>
-        <v>4.3599470781903236</v>
-      </c>
-      <c r="J27">
-        <f t="shared" si="1"/>
-        <v>-0.45949146911108468</v>
-      </c>
-      <c r="K27">
-        <f>_xlfn.T.TEST(4:4,$A$1:$DJK$17,2,3)</f>
         <v>1.4166305837829904E-41</v>
       </c>
       <c r="L27" t="b">
-        <f t="shared" ref="L27:L40" si="2">J27&lt;0.05</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="M27" t="str">
-        <f>IF(AND(L27,J27&gt;0),"\ora{"&amp;ROUND(J27,3)&amp;"}",IF(AND(L27,J27&lt;0),"\blu{"&amp;ROUND(J27,3)&amp;"}",ROUND(J27,3)))</f>
-        <v>\blu{-0.459}</v>
+        <f t="shared" si="3"/>
+        <v>\blu{-46}</v>
       </c>
     </row>
     <row r="28" spans="1:2975" x14ac:dyDescent="0.25">
@@ -66004,24 +66096,24 @@
         <v>12</v>
       </c>
       <c r="I28">
+        <f t="shared" si="1"/>
+        <v>9.3376911803444536</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="K28">
         <f t="shared" si="0"/>
-        <v>9.3376911803444536</v>
-      </c>
-      <c r="J28">
-        <f t="shared" si="1"/>
-        <v>0.15760619366904219</v>
-      </c>
-      <c r="K28">
-        <f>_xlfn.T.TEST(5:5,$A$1:$DJK$17,2,3)</f>
         <v>3.2194522581456746E-29</v>
       </c>
       <c r="L28" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M28">
-        <f>IF(AND(L28,J28&gt;0),"\ora{"&amp;ROUND(J28,3)&amp;"}",IF(AND(L28,J28&lt;0),"\blu{"&amp;ROUND(J28,3)&amp;"}",ROUND(J28,3)))</f>
-        <v>0.158</v>
+        <v>1</v>
+      </c>
+      <c r="M28" t="str">
+        <f t="shared" si="3"/>
+        <v>\ora{16}</v>
       </c>
     </row>
     <row r="29" spans="1:2975" x14ac:dyDescent="0.25">
@@ -66029,15 +66121,15 @@
         <v>11</v>
       </c>
       <c r="I29">
+        <f t="shared" si="1"/>
+        <v>8.4372800574368174</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="K29">
         <f t="shared" si="0"/>
-        <v>8.4372800574368174</v>
-      </c>
-      <c r="J29">
-        <f t="shared" si="1"/>
-        <v>4.5981010034737507E-2</v>
-      </c>
-      <c r="K29">
-        <f>_xlfn.T.TEST(6:6,$A$1:$DJK$17,2,3)</f>
         <v>1.1093570972311524E-6</v>
       </c>
       <c r="L29" t="b">
@@ -66045,8 +66137,8 @@
         <v>1</v>
       </c>
       <c r="M29" t="str">
-        <f>IF(AND(L29,J29&gt;0),"\ora{"&amp;ROUND(J29,3)&amp;"}",IF(AND(L29,J29&lt;0),"\blu{"&amp;ROUND(J29,3)&amp;"}",ROUND(J29,3)))</f>
-        <v>\ora{0.046}</v>
+        <f t="shared" si="3"/>
+        <v>\ora{5}</v>
       </c>
     </row>
     <row r="30" spans="1:2975" x14ac:dyDescent="0.25">
@@ -66054,24 +66146,24 @@
         <v>10</v>
       </c>
       <c r="I30">
+        <f t="shared" si="1"/>
+        <v>8.1222749690450549</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="K30">
         <f t="shared" si="0"/>
-        <v>8.1222749690450549</v>
-      </c>
-      <c r="J30">
-        <f t="shared" si="1"/>
-        <v>6.9294035597719256E-3</v>
-      </c>
-      <c r="K30">
-        <f>_xlfn.T.TEST(7:7,$A$1:$DJK$17,2,3)</f>
         <v>0.59914867574229302</v>
       </c>
       <c r="L30" t="b">
-        <f>J30&lt;0.05</f>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="3"/>
         <v>1</v>
-      </c>
-      <c r="M30" t="str">
-        <f>IF(AND(L30,J30&gt;0),"\ora{"&amp;ROUND(J30,3)&amp;"}",IF(AND(L30,J30&lt;0),"\blu{"&amp;ROUND(J30,3)&amp;"}",ROUND(J30,3)))</f>
-        <v>\ora{0.007}</v>
       </c>
     </row>
     <row r="31" spans="1:2975" x14ac:dyDescent="0.25">
@@ -66079,15 +66171,15 @@
         <v>9</v>
       </c>
       <c r="I31">
+        <f t="shared" si="1"/>
+        <v>5.852834801384919</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="4"/>
+        <v>-27</v>
+      </c>
+      <c r="K31">
         <f t="shared" si="0"/>
-        <v>5.852834801384919</v>
-      </c>
-      <c r="J31">
-        <f>(I31-$I$23)/$I$23</f>
-        <v>-0.27441616072432901</v>
-      </c>
-      <c r="K31">
-        <f>_xlfn.T.TEST(8:8,$A$1:$DJK$17,2,3)</f>
         <v>4.0725340140204074E-46</v>
       </c>
       <c r="L31" t="b">
@@ -66095,8 +66187,8 @@
         <v>1</v>
       </c>
       <c r="M31" t="str">
-        <f>IF(AND(L31,J31&gt;0),"\ora{"&amp;ROUND(J31,3)&amp;"}",IF(AND(L31,J31&lt;0),"\blu{"&amp;ROUND(J31,3)&amp;"}",ROUND(J31,3)))</f>
-        <v>\blu{-0.274}</v>
+        <f t="shared" si="3"/>
+        <v>\blu{-27}</v>
       </c>
     </row>
     <row r="32" spans="1:2975" x14ac:dyDescent="0.25">
@@ -66104,24 +66196,24 @@
         <v>8</v>
       </c>
       <c r="I32">
+        <f t="shared" si="1"/>
+        <v>7.9349505481263813</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="4"/>
+        <v>-2</v>
+      </c>
+      <c r="K32">
         <f t="shared" si="0"/>
-        <v>7.9349505481263813</v>
-      </c>
-      <c r="J32">
-        <f t="shared" si="1"/>
-        <v>-1.6293458033400182E-2</v>
-      </c>
-      <c r="K32">
-        <f>_xlfn.T.TEST(9:9,$A$1:$DJK$17,2,3)</f>
         <v>0.27664774300147565</v>
       </c>
       <c r="L32" t="b">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="M32" t="str">
-        <f>IF(AND(L32,J32&gt;0),"\ora{"&amp;ROUND(J32,3)&amp;"}",IF(AND(L32,J32&lt;0),"\blu{"&amp;ROUND(J32,3)&amp;"}",ROUND(J32,3)))</f>
-        <v>\blu{-0.016}</v>
+        <v>0</v>
+      </c>
+      <c r="M32">
+        <f t="shared" si="3"/>
+        <v>-2</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
@@ -66129,15 +66221,15 @@
         <v>7</v>
       </c>
       <c r="I33">
+        <f t="shared" si="1"/>
+        <v>6.8210863324482149</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="4"/>
+        <v>-15</v>
+      </c>
+      <c r="K33">
         <f t="shared" si="0"/>
-        <v>6.8210863324482149</v>
-      </c>
-      <c r="J33">
-        <f t="shared" si="1"/>
-        <v>-0.1543807100180809</v>
-      </c>
-      <c r="K33">
-        <f>_xlfn.T.TEST(10:10,$A$1:$DJK$17,2,3)</f>
         <v>5.6297822924057727E-28</v>
       </c>
       <c r="L33" t="b">
@@ -66145,8 +66237,8 @@
         <v>1</v>
       </c>
       <c r="M33" t="str">
-        <f>IF(AND(L33,J33&gt;0),"\ora{"&amp;ROUND(J33,3)&amp;"}",IF(AND(L33,J33&lt;0),"\blu{"&amp;ROUND(J33,3)&amp;"}",ROUND(J33,3)))</f>
-        <v>\blu{-0.154}</v>
+        <f t="shared" si="3"/>
+        <v>\blu{-15}</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
@@ -66154,24 +66246,24 @@
         <v>6</v>
       </c>
       <c r="I34">
+        <f t="shared" si="1"/>
+        <v>10.269756919754551</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="4"/>
+        <v>27</v>
+      </c>
+      <c r="K34">
         <f t="shared" si="0"/>
-        <v>10.269756919754551</v>
-      </c>
-      <c r="J34">
-        <f t="shared" si="1"/>
-        <v>0.27315564288610683</v>
-      </c>
-      <c r="K34">
-        <f>_xlfn.T.TEST(11:11,$A$1:$DJK$17,2,3)</f>
         <v>3.2273507831643851E-187</v>
       </c>
       <c r="L34" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M34">
-        <f>IF(AND(L34,J34&gt;0),"\ora{"&amp;ROUND(J34,3)&amp;"}",IF(AND(L34,J34&lt;0),"\blu{"&amp;ROUND(J34,3)&amp;"}",ROUND(J34,3)))</f>
-        <v>0.27300000000000002</v>
+        <v>1</v>
+      </c>
+      <c r="M34" t="str">
+        <f t="shared" si="3"/>
+        <v>\ora{27}</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
@@ -66179,15 +66271,15 @@
         <v>5</v>
       </c>
       <c r="I35">
+        <f t="shared" si="1"/>
+        <v>5.0997220123564384</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="4"/>
+        <v>-37</v>
+      </c>
+      <c r="K35">
         <f t="shared" si="0"/>
-        <v>5.0997220123564384</v>
-      </c>
-      <c r="J35">
-        <f t="shared" si="1"/>
-        <v>-0.36778057086308624</v>
-      </c>
-      <c r="K35">
-        <f>_xlfn.T.TEST(12:12,$A$1:$DJK$17,2,3)</f>
         <v>1.4533757606369977E-49</v>
       </c>
       <c r="L35" t="b">
@@ -66195,8 +66287,8 @@
         <v>1</v>
       </c>
       <c r="M35" t="str">
-        <f>IF(AND(L35,J35&gt;0),"\ora{"&amp;ROUND(J35,3)&amp;"}",IF(AND(L35,J35&lt;0),"\blu{"&amp;ROUND(J35,3)&amp;"}",ROUND(J35,3)))</f>
-        <v>\blu{-0.368}</v>
+        <f t="shared" si="3"/>
+        <v>\blu{-37}</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
@@ -66204,24 +66296,24 @@
         <v>4</v>
       </c>
       <c r="I36">
+        <f t="shared" si="1"/>
+        <v>8.2220219138004023</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="K36">
         <f t="shared" si="0"/>
-        <v>8.2220219138004023</v>
-      </c>
-      <c r="J36">
-        <f t="shared" si="1"/>
-        <v>1.9295167089348676E-2</v>
-      </c>
-      <c r="K36">
-        <f>_xlfn.T.TEST(13:13,$A$1:$DJK$17,2,3)</f>
         <v>0.10386417184814477</v>
       </c>
       <c r="L36" t="b">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="M36" t="str">
-        <f>IF(AND(L36,J36&gt;0),"\ora{"&amp;ROUND(J36,3)&amp;"}",IF(AND(L36,J36&lt;0),"\blu{"&amp;ROUND(J36,3)&amp;"}",ROUND(J36,3)))</f>
-        <v>\ora{0.019}</v>
+        <v>0</v>
+      </c>
+      <c r="M36">
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
@@ -66229,15 +66321,15 @@
         <v>3</v>
       </c>
       <c r="I37">
+        <f t="shared" si="1"/>
+        <v>6.23642545462382</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="4"/>
+        <v>-23</v>
+      </c>
+      <c r="K37">
         <f t="shared" si="0"/>
-        <v>6.23642545462382</v>
-      </c>
-      <c r="J37">
-        <f t="shared" si="1"/>
-        <v>-0.22686190909544557</v>
-      </c>
-      <c r="K37">
-        <f>_xlfn.T.TEST(14:14,$A$1:$DJK$17,2,3)</f>
         <v>3.2899041802173949E-25</v>
       </c>
       <c r="L37" t="b">
@@ -66245,8 +66337,8 @@
         <v>1</v>
       </c>
       <c r="M37" t="str">
-        <f>IF(AND(L37,J37&gt;0),"\ora{"&amp;ROUND(J37,3)&amp;"}",IF(AND(L37,J37&lt;0),"\blu{"&amp;ROUND(J37,3)&amp;"}",ROUND(J37,3)))</f>
-        <v>\blu{-0.227}</v>
+        <f t="shared" si="3"/>
+        <v>\blu{-23}</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
@@ -66254,24 +66346,24 @@
         <v>2</v>
       </c>
       <c r="I38">
+        <f t="shared" si="1"/>
+        <v>9.8391250648607933</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="4"/>
+        <v>22</v>
+      </c>
+      <c r="K38">
         <f t="shared" si="0"/>
-        <v>9.8391250648607933</v>
-      </c>
-      <c r="J38">
-        <f t="shared" si="1"/>
-        <v>0.21976962992119609</v>
-      </c>
-      <c r="K38">
-        <f>_xlfn.T.TEST(15:15,$A$1:$DJK$17,2,3)</f>
         <v>8.5154280910752009E-25</v>
       </c>
       <c r="L38" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M38">
-        <f>IF(AND(L38,J38&gt;0),"\ora{"&amp;ROUND(J38,3)&amp;"}",IF(AND(L38,J38&lt;0),"\blu{"&amp;ROUND(J38,3)&amp;"}",ROUND(J38,3)))</f>
-        <v>0.22</v>
+        <v>1</v>
+      </c>
+      <c r="M38" t="str">
+        <f t="shared" si="3"/>
+        <v>\ora{22}</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
@@ -66279,15 +66371,15 @@
         <v>1</v>
       </c>
       <c r="I39">
+        <f t="shared" si="1"/>
+        <v>2.6764515603323926</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="4"/>
+        <v>-67</v>
+      </c>
+      <c r="K39">
         <f t="shared" si="0"/>
-        <v>2.6764515603323926</v>
-      </c>
-      <c r="J39">
-        <f t="shared" si="1"/>
-        <v>-0.66819668337096816</v>
-      </c>
-      <c r="K39">
-        <f>_xlfn.T.TEST(16:16,$A$1:$DJK$17,2,3)</f>
         <v>2.7849638842812604E-303</v>
       </c>
       <c r="L39" t="b">
@@ -66295,8 +66387,8 @@
         <v>1</v>
       </c>
       <c r="M39" t="str">
-        <f>IF(AND(L39,J39&gt;0),"\ora{"&amp;ROUND(J39,3)&amp;"}",IF(AND(L39,J39&lt;0),"\blu{"&amp;ROUND(J39,3)&amp;"}",ROUND(J39,3)))</f>
-        <v>\blu{-0.668}</v>
+        <f t="shared" si="3"/>
+        <v>\blu{-67}</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
@@ -66308,20 +66400,20 @@
         <v>9.0913811262973745</v>
       </c>
       <c r="J40">
-        <f>(I40-$I$23)/$I$23</f>
-        <v>0.12707080342953148</v>
+        <f t="shared" si="4"/>
+        <v>13</v>
       </c>
       <c r="K40">
-        <f>_xlfn.T.TEST(17:17,$A$1:$DJK$17,2,3)</f>
+        <f t="shared" si="0"/>
         <v>2.3428920610519438E-55</v>
       </c>
       <c r="L40" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M40">
-        <f>IF(AND(L40,J40&gt;0),"\ora{"&amp;ROUND(J40,3)&amp;"}",IF(AND(L40,J40&lt;0),"\blu{"&amp;ROUND(J40,3)&amp;"}",ROUND(J40,3)))</f>
-        <v>0.127</v>
+        <v>1</v>
+      </c>
+      <c r="M40" t="str">
+        <f t="shared" si="3"/>
+        <v>\ora{13}</v>
       </c>
     </row>
   </sheetData>
@@ -66333,8 +66425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F86B412-AC88-43CF-9964-FEB6865D02B4}">
   <dimension ref="A1:PR40"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="N24" sqref="N24:N40"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -75039,6 +75131,12 @@
       <c r="K22" t="s">
         <v>69</v>
       </c>
+      <c r="N22" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="23" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -75048,11 +75146,16 @@
         <f>AVERAGE(A1:DJK17)</f>
         <v>5.5972693640028011</v>
       </c>
-      <c r="N23" t="s">
-        <v>190</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>189</v>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="N23" t="str">
+        <f t="shared" ref="L23:N40" si="0">IF(Q23&lt;0.05,"Yes","No")</f>
+        <v>Yes</v>
+      </c>
+      <c r="Q23">
+        <f>_xlfn.T.TEST('Beam MCSP overlap raw dcgs'!1:17,'Beam MCSP all raw dcgs'!1:17,2,3)</f>
+        <v>4.3752295140644669E-282</v>
       </c>
     </row>
     <row r="24" spans="1:86" x14ac:dyDescent="0.25">
@@ -75064,23 +75167,23 @@
         <v>6.8430250362219347</v>
       </c>
       <c r="J24">
-        <f>(I24-$I$23)/$I$23</f>
-        <v>0.22256489570268789</v>
+        <f>100*ROUND((I24-$I$23)/$I$23,2)</f>
+        <v>22</v>
       </c>
       <c r="K24">
-        <f>_xlfn.T.TEST(1:1,$A$1:$DJK$17,2,3)</f>
+        <f t="shared" ref="K24:K40" si="1">_xlfn.T.TEST(1:1,$A$1:$DJK$17,2,3)</f>
         <v>9.2794491286855467E-14</v>
       </c>
       <c r="L24" t="b">
-        <f>J24&lt;0.05</f>
-        <v>0</v>
-      </c>
-      <c r="M24">
-        <f>IF(AND(L24,J24&gt;0),"\ora{"&amp;ROUND(J24,3)&amp;"}",IF(AND(L24,J24&lt;0),"\blu{"&amp;ROUND(J24,3)&amp;"}",ROUND(J24,3)))</f>
-        <v>0.223</v>
+        <f>K24&lt;0.05</f>
+        <v>1</v>
+      </c>
+      <c r="M24" t="str">
+        <f>IF(AND(L24,J24&gt;0),"\ora{"&amp;J24&amp;"}",IF(AND(L24,J24&lt;0),"\blu{"&amp;J24&amp;"}",J24))</f>
+        <v>\ora{22}</v>
       </c>
       <c r="N24" t="str">
-        <f>IF(Q24&lt;0.05,"Yes","No")</f>
+        <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
       <c r="Q24">
@@ -75093,27 +75196,27 @@
         <v>15</v>
       </c>
       <c r="I25">
-        <f t="shared" ref="I25:I39" si="0">AVERAGE(2:2)</f>
+        <f t="shared" ref="I25:I39" si="2">AVERAGE(2:2)</f>
         <v>4.4677419593915282</v>
       </c>
       <c r="J25">
-        <f t="shared" ref="J25:J39" si="1">(I25-$I$23)/$I$23</f>
-        <v>-0.20179972253533082</v>
+        <f t="shared" ref="J25:J40" si="3">100*ROUND((I25-$I$23)/$I$23,2)</f>
+        <v>-20</v>
       </c>
       <c r="K25">
-        <f>_xlfn.T.TEST(2:2,$A$1:$DJK$17,2,3)</f>
+        <f t="shared" si="1"/>
         <v>7.6015199626303947E-8</v>
       </c>
       <c r="L25" t="b">
-        <f>J25&lt;0.05</f>
+        <f t="shared" ref="L25:L40" si="4">K25&lt;0.05</f>
         <v>1</v>
       </c>
       <c r="M25" t="str">
-        <f>IF(AND(L25,J25&gt;0),"\ora{"&amp;ROUND(J25,3)&amp;"}",IF(AND(L25,J25&lt;0),"\blu{"&amp;ROUND(J25,3)&amp;"}",ROUND(J25,3)))</f>
-        <v>\blu{-0.202}</v>
+        <f t="shared" ref="M25:M40" si="5">IF(AND(L25,J25&gt;0),"\ora{"&amp;J25&amp;"}",IF(AND(L25,J25&lt;0),"\blu{"&amp;J25&amp;"}",J25))</f>
+        <v>\blu{-20}</v>
       </c>
       <c r="N25" t="str">
-        <f>IF(Q25&lt;0.05,"Yes","No")</f>
+        <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
       <c r="Q25">
@@ -75126,27 +75229,27 @@
         <v>14</v>
       </c>
       <c r="I26">
+        <f t="shared" si="2"/>
+        <v>3.9758853697661558</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="3"/>
+        <v>-28.999999999999996</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="1"/>
+        <v>1.9200799869147907E-20</v>
+      </c>
+      <c r="L26" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M26" t="str">
+        <f t="shared" si="5"/>
+        <v>\blu{-29}</v>
+      </c>
+      <c r="N26" t="str">
         <f t="shared" si="0"/>
-        <v>3.9758853697661558</v>
-      </c>
-      <c r="J26">
-        <f t="shared" si="1"/>
-        <v>-0.28967410513849873</v>
-      </c>
-      <c r="K26">
-        <f>_xlfn.T.TEST(3:3,$A$1:$DJK$17,2,3)</f>
-        <v>1.9200799869147907E-20</v>
-      </c>
-      <c r="L26" t="b">
-        <f>J26&lt;0.05</f>
-        <v>1</v>
-      </c>
-      <c r="M26" t="str">
-        <f>IF(AND(L26,J26&gt;0),"\ora{"&amp;ROUND(J26,3)&amp;"}",IF(AND(L26,J26&lt;0),"\blu{"&amp;ROUND(J26,3)&amp;"}",ROUND(J26,3)))</f>
-        <v>\blu{-0.29}</v>
-      </c>
-      <c r="N26" t="str">
-        <f>IF(Q26&lt;0.05,"Yes","No")</f>
         <v>Yes</v>
       </c>
       <c r="Q26">
@@ -75159,27 +75262,27 @@
         <v>13</v>
       </c>
       <c r="I27">
+        <f t="shared" si="2"/>
+        <v>3.6669327969756744</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="3"/>
+        <v>-34</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="1"/>
+        <v>1.0331213972196151E-10</v>
+      </c>
+      <c r="L27" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M27" t="str">
+        <f t="shared" si="5"/>
+        <v>\blu{-34}</v>
+      </c>
+      <c r="N27" t="str">
         <f t="shared" si="0"/>
-        <v>3.6669327969756744</v>
-      </c>
-      <c r="J27">
-        <f t="shared" si="1"/>
-        <v>-0.34487112223712529</v>
-      </c>
-      <c r="K27">
-        <f>_xlfn.T.TEST(4:4,$A$1:$DJK$17,2,3)</f>
-        <v>1.0331213972196151E-10</v>
-      </c>
-      <c r="L27" t="b">
-        <f t="shared" ref="L27:L40" si="2">J27&lt;0.05</f>
-        <v>1</v>
-      </c>
-      <c r="M27" t="str">
-        <f>IF(AND(L27,J27&gt;0),"\ora{"&amp;ROUND(J27,3)&amp;"}",IF(AND(L27,J27&lt;0),"\blu{"&amp;ROUND(J27,3)&amp;"}",ROUND(J27,3)))</f>
-        <v>\blu{-0.345}</v>
-      </c>
-      <c r="N27" t="str">
-        <f>IF(Q27&lt;0.05,"Yes","No")</f>
         <v>Yes</v>
       </c>
       <c r="Q27">
@@ -75192,27 +75295,27 @@
         <v>12</v>
       </c>
       <c r="I28">
+        <f t="shared" si="2"/>
+        <v>7.6720359017048683</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="3"/>
+        <v>37</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="1"/>
+        <v>9.2058984622945683E-20</v>
+      </c>
+      <c r="L28" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M28" t="str">
+        <f t="shared" si="5"/>
+        <v>\ora{37}</v>
+      </c>
+      <c r="N28" t="str">
         <f t="shared" si="0"/>
-        <v>7.6720359017048683</v>
-      </c>
-      <c r="J28">
-        <f t="shared" si="1"/>
-        <v>0.3706747706382188</v>
-      </c>
-      <c r="K28">
-        <f>_xlfn.T.TEST(5:5,$A$1:$DJK$17,2,3)</f>
-        <v>9.2058984622945683E-20</v>
-      </c>
-      <c r="L28" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M28">
-        <f>IF(AND(L28,J28&gt;0),"\ora{"&amp;ROUND(J28,3)&amp;"}",IF(AND(L28,J28&lt;0),"\blu{"&amp;ROUND(J28,3)&amp;"}",ROUND(J28,3)))</f>
-        <v>0.371</v>
-      </c>
-      <c r="N28" t="str">
-        <f>IF(Q28&lt;0.05,"Yes","No")</f>
         <v>Yes</v>
       </c>
       <c r="Q28">
@@ -75225,27 +75328,27 @@
         <v>11</v>
       </c>
       <c r="I29">
+        <f t="shared" si="2"/>
+        <v>7.266461055114263</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="1"/>
+        <v>1.3221958086966967E-24</v>
+      </c>
+      <c r="L29" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M29" t="str">
+        <f t="shared" si="5"/>
+        <v>\ora{30}</v>
+      </c>
+      <c r="N29" t="str">
         <f t="shared" si="0"/>
-        <v>7.266461055114263</v>
-      </c>
-      <c r="J29">
-        <f t="shared" si="1"/>
-        <v>0.29821535869729254</v>
-      </c>
-      <c r="K29">
-        <f>_xlfn.T.TEST(6:6,$A$1:$DJK$17,2,3)</f>
-        <v>1.3221958086966967E-24</v>
-      </c>
-      <c r="L29" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M29">
-        <f>IF(AND(L29,J29&gt;0),"\ora{"&amp;ROUND(J29,3)&amp;"}",IF(AND(L29,J29&lt;0),"\blu{"&amp;ROUND(J29,3)&amp;"}",ROUND(J29,3)))</f>
-        <v>0.29799999999999999</v>
-      </c>
-      <c r="N29" t="str">
-        <f>IF(Q29&lt;0.05,"Yes","No")</f>
         <v>Yes</v>
       </c>
       <c r="Q29">
@@ -75258,27 +75361,27 @@
         <v>10</v>
       </c>
       <c r="I30">
+        <f t="shared" si="2"/>
+        <v>7.7403307054998551</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="3"/>
+        <v>38</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="1"/>
+        <v>2.4818201937064209E-24</v>
+      </c>
+      <c r="L30" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M30" t="str">
+        <f t="shared" si="5"/>
+        <v>\ora{38}</v>
+      </c>
+      <c r="N30" t="str">
         <f t="shared" si="0"/>
-        <v>7.7403307054998551</v>
-      </c>
-      <c r="J30">
-        <f t="shared" si="1"/>
-        <v>0.38287622090863188</v>
-      </c>
-      <c r="K30">
-        <f>_xlfn.T.TEST(7:7,$A$1:$DJK$17,2,3)</f>
-        <v>2.4818201937064209E-24</v>
-      </c>
-      <c r="L30" t="b">
-        <f>J30&lt;0.05</f>
-        <v>0</v>
-      </c>
-      <c r="M30">
-        <f>IF(AND(L30,J30&gt;0),"\ora{"&amp;ROUND(J30,3)&amp;"}",IF(AND(L30,J30&lt;0),"\blu{"&amp;ROUND(J30,3)&amp;"}",ROUND(J30,3)))</f>
-        <v>0.38300000000000001</v>
-      </c>
-      <c r="N30" t="str">
-        <f>IF(Q30&lt;0.05,"Yes","No")</f>
         <v>No</v>
       </c>
       <c r="Q30">
@@ -75291,27 +75394,27 @@
         <v>9</v>
       </c>
       <c r="I31">
+        <f t="shared" si="2"/>
+        <v>4.6443255395767364</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="3"/>
+        <v>-17</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="1"/>
+        <v>1.3827773968962291E-6</v>
+      </c>
+      <c r="L31" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M31" t="str">
+        <f t="shared" si="5"/>
+        <v>\blu{-17}</v>
+      </c>
+      <c r="N31" t="str">
         <f t="shared" si="0"/>
-        <v>4.6443255395767364</v>
-      </c>
-      <c r="J31">
-        <f>(I31-$I$23)/$I$23</f>
-        <v>-0.17025155704577016</v>
-      </c>
-      <c r="K31">
-        <f>_xlfn.T.TEST(8:8,$A$1:$DJK$17,2,3)</f>
-        <v>1.3827773968962291E-6</v>
-      </c>
-      <c r="L31" t="b">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="M31" t="str">
-        <f>IF(AND(L31,J31&gt;0),"\ora{"&amp;ROUND(J31,3)&amp;"}",IF(AND(L31,J31&lt;0),"\blu{"&amp;ROUND(J31,3)&amp;"}",ROUND(J31,3)))</f>
-        <v>\blu{-0.17}</v>
-      </c>
-      <c r="N31" t="str">
-        <f>IF(Q31&lt;0.05,"Yes","No")</f>
         <v>Yes</v>
       </c>
       <c r="Q31">
@@ -75324,27 +75427,27 @@
         <v>8</v>
       </c>
       <c r="I32">
+        <f t="shared" si="2"/>
+        <v>4.6156940107140123</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="3"/>
+        <v>-18</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="1"/>
+        <v>1.0520507184378385E-7</v>
+      </c>
+      <c r="L32" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M32" t="str">
+        <f t="shared" si="5"/>
+        <v>\blu{-18}</v>
+      </c>
+      <c r="N32" t="str">
         <f t="shared" si="0"/>
-        <v>4.6156940107140123</v>
-      </c>
-      <c r="J32">
-        <f t="shared" si="1"/>
-        <v>-0.17536682433071799</v>
-      </c>
-      <c r="K32">
-        <f>_xlfn.T.TEST(9:9,$A$1:$DJK$17,2,3)</f>
-        <v>1.0520507184378385E-7</v>
-      </c>
-      <c r="L32" t="b">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="M32" t="str">
-        <f>IF(AND(L32,J32&gt;0),"\ora{"&amp;ROUND(J32,3)&amp;"}",IF(AND(L32,J32&lt;0),"\blu{"&amp;ROUND(J32,3)&amp;"}",ROUND(J32,3)))</f>
-        <v>\blu{-0.175}</v>
-      </c>
-      <c r="N32" t="str">
-        <f>IF(Q32&lt;0.05,"Yes","No")</f>
         <v>Yes</v>
       </c>
       <c r="Q32">
@@ -75357,27 +75460,27 @@
         <v>7</v>
       </c>
       <c r="I33">
+        <f t="shared" si="2"/>
+        <v>5.7470328225148117</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="1"/>
+        <v>0.40295519690548076</v>
+      </c>
+      <c r="L33" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M33">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="N33" t="str">
         <f t="shared" si="0"/>
-        <v>5.7470328225148117</v>
-      </c>
-      <c r="J33">
-        <f t="shared" si="1"/>
-        <v>2.6756521577319559E-2</v>
-      </c>
-      <c r="K33">
-        <f>_xlfn.T.TEST(10:10,$A$1:$DJK$17,2,3)</f>
-        <v>0.40295519690548076</v>
-      </c>
-      <c r="L33" t="b">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="M33" t="str">
-        <f>IF(AND(L33,J33&gt;0),"\ora{"&amp;ROUND(J33,3)&amp;"}",IF(AND(L33,J33&lt;0),"\blu{"&amp;ROUND(J33,3)&amp;"}",ROUND(J33,3)))</f>
-        <v>\ora{0.027}</v>
-      </c>
-      <c r="N33" t="str">
-        <f>IF(Q33&lt;0.05,"Yes","No")</f>
         <v>Yes</v>
       </c>
       <c r="Q33">
@@ -75390,27 +75493,27 @@
         <v>6</v>
       </c>
       <c r="I34">
+        <f t="shared" si="2"/>
+        <v>2.4667761900182841</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="3"/>
+        <v>-56.000000000000007</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="1"/>
+        <v>1.8954873358995736E-6</v>
+      </c>
+      <c r="L34" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M34" t="str">
+        <f t="shared" si="5"/>
+        <v>\blu{-56}</v>
+      </c>
+      <c r="N34" t="str">
         <f t="shared" si="0"/>
-        <v>2.4667761900182841</v>
-      </c>
-      <c r="J34">
-        <f t="shared" si="1"/>
-        <v>-0.55928935529123669</v>
-      </c>
-      <c r="K34">
-        <f>_xlfn.T.TEST(11:11,$A$1:$DJK$17,2,3)</f>
-        <v>1.8954873358995736E-6</v>
-      </c>
-      <c r="L34" t="b">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="M34" t="str">
-        <f>IF(AND(L34,J34&gt;0),"\ora{"&amp;ROUND(J34,3)&amp;"}",IF(AND(L34,J34&lt;0),"\blu{"&amp;ROUND(J34,3)&amp;"}",ROUND(J34,3)))</f>
-        <v>\blu{-0.559}</v>
-      </c>
-      <c r="N34" t="str">
-        <f>IF(Q34&lt;0.05,"Yes","No")</f>
         <v>Yes</v>
       </c>
       <c r="Q34">
@@ -75423,27 +75526,27 @@
         <v>5</v>
       </c>
       <c r="I35">
+        <f t="shared" si="2"/>
+        <v>4.0136388428633794</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="3"/>
+        <v>-28.000000000000004</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="1"/>
+        <v>2.8513673781584609E-7</v>
+      </c>
+      <c r="L35" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M35" t="str">
+        <f t="shared" si="5"/>
+        <v>\blu{-28}</v>
+      </c>
+      <c r="N35" t="str">
         <f t="shared" si="0"/>
-        <v>4.0136388428633794</v>
-      </c>
-      <c r="J35">
-        <f t="shared" si="1"/>
-        <v>-0.28292912456993363</v>
-      </c>
-      <c r="K35">
-        <f>_xlfn.T.TEST(12:12,$A$1:$DJK$17,2,3)</f>
-        <v>2.8513673781584609E-7</v>
-      </c>
-      <c r="L35" t="b">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="M35" t="str">
-        <f>IF(AND(L35,J35&gt;0),"\ora{"&amp;ROUND(J35,3)&amp;"}",IF(AND(L35,J35&lt;0),"\blu{"&amp;ROUND(J35,3)&amp;"}",ROUND(J35,3)))</f>
-        <v>\blu{-0.283}</v>
-      </c>
-      <c r="N35" t="str">
-        <f>IF(Q35&lt;0.05,"Yes","No")</f>
         <v>Yes</v>
       </c>
       <c r="Q35">
@@ -75456,27 +75559,27 @@
         <v>4</v>
       </c>
       <c r="I36">
+        <f t="shared" si="2"/>
+        <v>5.2414180480041113</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="3"/>
+        <v>-6</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="1"/>
+        <v>8.2416815315318956E-2</v>
+      </c>
+      <c r="L36" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M36">
+        <f t="shared" si="5"/>
+        <v>-6</v>
+      </c>
+      <c r="N36" t="str">
         <f t="shared" si="0"/>
-        <v>5.2414180480041113</v>
-      </c>
-      <c r="J36">
-        <f t="shared" si="1"/>
-        <v>-6.3575878317960424E-2</v>
-      </c>
-      <c r="K36">
-        <f>_xlfn.T.TEST(13:13,$A$1:$DJK$17,2,3)</f>
-        <v>8.2416815315318956E-2</v>
-      </c>
-      <c r="L36" t="b">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="M36" t="str">
-        <f>IF(AND(L36,J36&gt;0),"\ora{"&amp;ROUND(J36,3)&amp;"}",IF(AND(L36,J36&lt;0),"\blu{"&amp;ROUND(J36,3)&amp;"}",ROUND(J36,3)))</f>
-        <v>\blu{-0.064}</v>
-      </c>
-      <c r="N36" t="str">
-        <f>IF(Q36&lt;0.05,"Yes","No")</f>
         <v>Yes</v>
       </c>
       <c r="Q36">
@@ -75489,27 +75592,27 @@
         <v>3</v>
       </c>
       <c r="I37">
+        <f t="shared" si="2"/>
+        <v>5.0497655156784367</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="3"/>
+        <v>-10</v>
+      </c>
+      <c r="K37">
+        <f t="shared" si="1"/>
+        <v>0.10510692038516074</v>
+      </c>
+      <c r="L37" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M37">
+        <f t="shared" si="5"/>
+        <v>-10</v>
+      </c>
+      <c r="N37" t="str">
         <f t="shared" si="0"/>
-        <v>5.0497655156784367</v>
-      </c>
-      <c r="J37">
-        <f t="shared" si="1"/>
-        <v>-9.7816240870141971E-2</v>
-      </c>
-      <c r="K37">
-        <f>_xlfn.T.TEST(14:14,$A$1:$DJK$17,2,3)</f>
-        <v>0.10510692038516074</v>
-      </c>
-      <c r="L37" t="b">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="M37" t="str">
-        <f>IF(AND(L37,J37&gt;0),"\ora{"&amp;ROUND(J37,3)&amp;"}",IF(AND(L37,J37&lt;0),"\blu{"&amp;ROUND(J37,3)&amp;"}",ROUND(J37,3)))</f>
-        <v>\blu{-0.098}</v>
-      </c>
-      <c r="N37" t="str">
-        <f>IF(Q37&lt;0.05,"Yes","No")</f>
         <v>Yes</v>
       </c>
       <c r="Q37">
@@ -75522,27 +75625,27 @@
         <v>2</v>
       </c>
       <c r="I38">
+        <f t="shared" si="2"/>
+        <v>2.4931642859137186</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="3"/>
+        <v>-55.000000000000007</v>
+      </c>
+      <c r="K38">
+        <f t="shared" si="1"/>
+        <v>3.0946748416930134E-6</v>
+      </c>
+      <c r="L38" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M38" t="str">
+        <f t="shared" si="5"/>
+        <v>\blu{-55}</v>
+      </c>
+      <c r="N38" t="str">
         <f t="shared" si="0"/>
-        <v>2.4931642859137186</v>
-      </c>
-      <c r="J38">
-        <f t="shared" si="1"/>
-        <v>-0.55457489647581115</v>
-      </c>
-      <c r="K38">
-        <f>_xlfn.T.TEST(15:15,$A$1:$DJK$17,2,3)</f>
-        <v>3.0946748416930134E-6</v>
-      </c>
-      <c r="L38" t="b">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="M38" t="str">
-        <f>IF(AND(L38,J38&gt;0),"\ora{"&amp;ROUND(J38,3)&amp;"}",IF(AND(L38,J38&lt;0),"\blu{"&amp;ROUND(J38,3)&amp;"}",ROUND(J38,3)))</f>
-        <v>\blu{-0.555}</v>
-      </c>
-      <c r="N38" t="str">
-        <f>IF(Q38&lt;0.05,"Yes","No")</f>
         <v>Yes</v>
       </c>
       <c r="Q38">
@@ -75555,27 +75658,27 @@
         <v>1</v>
       </c>
       <c r="I39">
+        <f t="shared" si="2"/>
+        <v>2.8103416848946741</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="3"/>
+        <v>-50</v>
+      </c>
+      <c r="K39">
+        <f t="shared" si="1"/>
+        <v>6.6698384776798324E-79</v>
+      </c>
+      <c r="L39" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M39" t="str">
+        <f t="shared" si="5"/>
+        <v>\blu{-50}</v>
+      </c>
+      <c r="N39" t="str">
         <f t="shared" si="0"/>
-        <v>2.8103416848946741</v>
-      </c>
-      <c r="J39">
-        <f t="shared" si="1"/>
-        <v>-0.49790844389791855</v>
-      </c>
-      <c r="K39">
-        <f>_xlfn.T.TEST(16:16,$A$1:$DJK$17,2,3)</f>
-        <v>6.6698384776798324E-79</v>
-      </c>
-      <c r="L39" t="b">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="M39" t="str">
-        <f>IF(AND(L39,J39&gt;0),"\ora{"&amp;ROUND(J39,3)&amp;"}",IF(AND(L39,J39&lt;0),"\blu{"&amp;ROUND(J39,3)&amp;"}",ROUND(J39,3)))</f>
-        <v>\blu{-0.498}</v>
-      </c>
-      <c r="N39" t="str">
-        <f>IF(Q39&lt;0.05,"Yes","No")</f>
         <v>No</v>
       </c>
       <c r="Q39">
@@ -75592,23 +75695,23 @@
         <v>2.4152210628280666</v>
       </c>
       <c r="J40">
-        <f>(I40-$I$23)/$I$23</f>
-        <v>-0.56850011929730349</v>
+        <f t="shared" si="3"/>
+        <v>-56.999999999999993</v>
       </c>
       <c r="K40">
-        <f>_xlfn.T.TEST(17:17,$A$1:$DJK$17,2,3)</f>
+        <f t="shared" si="1"/>
         <v>3.3713232452749535E-24</v>
       </c>
       <c r="L40" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M40" t="str">
-        <f>IF(AND(L40,J40&gt;0),"\ora{"&amp;ROUND(J40,3)&amp;"}",IF(AND(L40,J40&lt;0),"\blu{"&amp;ROUND(J40,3)&amp;"}",ROUND(J40,3)))</f>
-        <v>\blu{-0.569}</v>
+        <f t="shared" si="5"/>
+        <v>\blu{-57}</v>
       </c>
       <c r="N40" t="str">
-        <f>IF(Q40&lt;0.05,"Yes","No")</f>
+        <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
       <c r="Q40">

</xml_diff>